<commit_message>
154963 Change test harness template url and save product upload details
</commit_message>
<xml_diff>
--- a/Marketplace/LANSA Scalable License/AWS/2016-08-17.xlsx
+++ b/Marketplace/LANSA Scalable License/AWS/2016-08-17.xlsx
@@ -6410,9 +6410,9 @@
   </sheetPr>
   <dimension ref="A1:JU9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO9" sqref="AO9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15.95" customHeight="1"/>
@@ -14157,7 +14157,7 @@
     <hyperlink ref="S6" r:id="rId5"/>
     <hyperlink ref="T6" r:id="rId6"/>
     <hyperlink ref="V6" r:id="rId7"/>
-    <hyperlink ref="W9"/>
+    <hyperlink ref="W9" display="http://www.lansa.com/support/register/helpdesk.htm_x000a_The LANSA Product Support team is highly qualified to provide timely, accurate information and assistance on the entire suite of LANSA products. From answering simple installation questions to troubleshoo"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -15088,18 +15088,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15119,14 +15119,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B5DC2E0-0871-44B1-89B4-ACA1409A331A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{926ACF4F-A83A-4655-A95E-1B7425DC877E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -15139,4 +15131,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B5DC2E0-0871-44B1-89B4-ACA1409A331A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>